<commit_message>
as of 20 june 2025 9:15 am-Friday before market start
</commit_message>
<xml_diff>
--- a/ORDER_MGMT/order_files/Filtered_data.xlsx
+++ b/ORDER_MGMT/order_files/Filtered_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,44 +522,44 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:22 PM</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>KAYNESEQ</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
         <v>6</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>18 JUN 2025 09:01:00 AM</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>NSE</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>GRSEEQ</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>16</v>
-      </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>3283</v>
+        <v>5796</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -581,25 +581,25 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Executed</t>
+          <t>Expired</t>
         </is>
       </c>
       <c r="P2" t="n">
-        <v>20250618004944</v>
+        <v>20250618040210</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>'1100000000161155</t>
+          <t>'1200000012497182</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>18 JUN 2025 09:01:00 AM</t>
+          <t>18 JUN 2025 04:26:13 PM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -609,7 +609,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>GRSEEQ</t>
+          <t>NAM-INDIAEQ</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>3217</v>
+        <v>784</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
@@ -654,25 +654,25 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Executed</t>
+          <t>Expired</t>
         </is>
       </c>
       <c r="P3" t="n">
-        <v>20250618004898</v>
+        <v>20250618004974</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>'1100000000160719</t>
+          <t>'1200000000118192</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>18 JUN 2025 09:00:59 AM</t>
+          <t>18 JUN 2025 04:26:22 PM</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -696,46 +696,1725 @@
         </is>
       </c>
       <c r="G4" t="n">
+        <v>50</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1274</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P4" t="n">
+        <v>20250618004973</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>'1200000000119038</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:31 PM</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>VBLEQ</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>80</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>482</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P5" t="n">
+        <v>20250618004946</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>'1300000000146512</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:18 PM</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>INDHOTELEQ</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>100</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>783</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P6" t="n">
+        <v>20250618004945</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>'1100000000162627</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:34 PM</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>JUSTDIALEQ</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>60</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>935</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P7" t="n">
+        <v>20250618004928</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>'1100000000161026</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:34 PM</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>JUSTDIALEQ</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>50</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>926</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P8" t="n">
+        <v>20250618004927</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>'1100000000162417</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:34 PM</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>JUSTDIALEQ</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>40</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>914</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P9" t="n">
+        <v>20250618004926</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>'1100000000161010</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:18 PM</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>INDHOTELEQ</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>45</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>774</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P10" t="n">
+        <v>20250618004899</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>'1100000000162105</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>12</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:13 PM</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>NAM-INDIAEQ</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>35</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>774</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P11" t="n">
+        <v>20250618004897</v>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>'1200000000118525</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>13</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:18 PM</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>BDLEQ</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>25</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2080</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P12" t="n">
+        <v>20250618004896</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>'1000000000109275</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>14</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:27 PM</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>CDSLEQ</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>11</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1822</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P13" t="n">
+        <v>20250618004847</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>'1000000000109787</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>16</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:22 PM</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>IRCONEQ</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>100</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>214</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P14" t="n">
+        <v>20250618004827</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>'1100000000161308</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>17</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:23 PM</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>IRCONEQ</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>140</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>226</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P15" t="n">
+        <v>20250618004826</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>'1100000000160023</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>18</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:20 PM</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>IRFCEQ</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>100</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>148.5</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P16" t="n">
+        <v>20250618004825</v>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>'1100000000161290</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>19</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:25 PM</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>RVNLEQ</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>80</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>419</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P17" t="n">
+        <v>20250618004649</v>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>'1300000000145404</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
         <v>20</v>
       </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>20</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1240</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Reg lot</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>CASH</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>Executed</t>
-        </is>
-      </c>
-      <c r="P4" t="n">
-        <v>20250618004846</v>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>'1200000000117471</t>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 09:00:57 AM</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>IGILEQ</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>30</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>408</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Rejected</t>
+        </is>
+      </c>
+      <c r="P18" t="n">
+        <v>20250618002878</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>'1100000000157905</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>21</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 09:00:58 AM</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>ZENTECEQ</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>10</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2065</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Rejected</t>
+        </is>
+      </c>
+      <c r="P19" t="n">
+        <v>20250618002857</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>'1300000000145033</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>22</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:17 PM</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>RAILTELEQ</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>70</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>474</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P20" t="n">
+        <v>20250618002832</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>'1300000000143725</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>23</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:17 PM</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>RAILTELEQ</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>60</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>468</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P21" t="n">
+        <v>20250618002734</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>'1300000000142987</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>24</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:17 PM</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>RAILTELEQ</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>60</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>448</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P22" t="n">
+        <v>20250618002684</v>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>'1300000000142573</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>25</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:33 PM</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>IGILEQ</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>50</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>388.5</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P23" t="n">
+        <v>20250618000904</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>'1100000000143532</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>26</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:15 PM</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>BELEQ</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>100</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>408</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P24" t="n">
+        <v>20250618000903</v>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>'1000000000100226</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>27</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:29 PM</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>TECHMEQ</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>10</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1743</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P25" t="n">
+        <v>20250618000902</v>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>'1300000000133178</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>28</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:29 PM</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>SOLARINDSEQ</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>17690</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P26" t="n">
+        <v>20250618000901</v>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>'1300000000134688</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>29</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>18 JUN 2025 04:26:32 PM</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>IREDAEQ</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>100</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>177</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Reg lot</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Expired</t>
+        </is>
+      </c>
+      <c r="P27" t="n">
+        <v>20250618000900</v>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>cu</t>
         </is>
       </c>
     </row>

</xml_diff>